<commit_message>
Sua doi lan 2
</commit_message>
<xml_diff>
--- a/product_backlog.xlsx
+++ b/product_backlog.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\15CNTN\HK2\NhapmonCNTT2\DOAN1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+  <si>
+    <t>PRODUCT BACKLOG OF "WEBSITE SUPPORT REGISTER CAMP"</t>
+  </si>
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -32,12 +35,12 @@
     <t>As a / an</t>
   </si>
   <si>
+    <t>I want to…</t>
+  </si>
+  <si>
     <t>so that…</t>
   </si>
   <si>
-    <t>I want to…</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -56,127 +59,70 @@
     <t>priority</t>
   </si>
   <si>
-    <t>The analyst/PO</t>
-  </si>
-  <si>
-    <t>1 hour</t>
-  </si>
-  <si>
-    <t>Scrum master</t>
-  </si>
-  <si>
-    <t>3 hour</t>
-  </si>
-  <si>
-    <t>Development Team</t>
+    <t>Website Visitor</t>
+  </si>
+  <si>
+    <t>Thấy được giao diện, bố cục trang web</t>
+  </si>
+  <si>
+    <t>Hiểu được trang web hỗ trợ gì cho người dùng</t>
+  </si>
+  <si>
+    <t>Thấy được sự tiện lợi khi đăng kí cắm trại qua Web</t>
+  </si>
+  <si>
+    <t>Thuận tiện trong việc quản lí cũng như triển khai</t>
+  </si>
+  <si>
+    <t>Đăng nhập</t>
+  </si>
+  <si>
+    <t>Giúp quản lí được một hoạt động cắm trại: trại sinh và BTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trang đăng kí cho trại sinh </t>
+  </si>
+  <si>
+    <t>Giúp trại sinh đăng kí và đóng tiền thuận tiện</t>
+  </si>
+  <si>
+    <t>Trang quản lí cho BTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giúp ban tổ chức quản lí thuận tiện hơn việc đăng kí </t>
+  </si>
+  <si>
+    <t>Hệ thống gửi email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giúp tương tác với người dùng tốt hơn </t>
+  </si>
+  <si>
+    <t>1 week</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>2 days</t>
   </si>
   <si>
     <t>1 day</t>
   </si>
   <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>2 hour</t>
-  </si>
-  <si>
-    <t>1 week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PO + Scrum Master + Development Team + Tester </t>
-  </si>
-  <si>
-    <t>HTHieu + HVNHuy + DTPhong + DBKien + DTLam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 hour </t>
-  </si>
-  <si>
-    <t>HVNHuy + DTPhong + DBKien</t>
-  </si>
-  <si>
-    <t>Scrum Master + Development Team + Tester</t>
-  </si>
-  <si>
-    <t>HVNHuy + DTPhong + DBKien + DTLam</t>
-  </si>
-  <si>
-    <t>1 hour / 1 day</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 day + 16 hour </t>
-  </si>
-  <si>
-    <t>PRODUCT BACKLOG OF "WEBSITE SUPPORT REGISTER CAMP"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analysis Requirements and design website </t>
-  </si>
-  <si>
-    <t>Set up Product Backlog &amp; Sprint Backlog</t>
-  </si>
-  <si>
-    <t>Design UI</t>
-  </si>
-  <si>
-    <t>Check UI</t>
-  </si>
-  <si>
-    <t>Building registration function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scrum meeting </t>
-  </si>
-  <si>
-    <t>Sprint: Sum up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint: Meeting and Improve </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set up Product Backlog &amp; Sprint Backlog and Development Team succesful </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scrum meeting and update status of the process everyday. </t>
-  </si>
-  <si>
-    <t>Sum up the process of sprint. If it is over deadline, we have to skip and complete in next sprint</t>
-  </si>
-  <si>
-    <t>Collectively the requirements needed to create a register for camp sites. To be brief idea of the components required in the website</t>
-  </si>
-  <si>
-    <t>Create login interface and site registration</t>
-  </si>
-  <si>
-    <t>Build registration function for "organizers"</t>
-  </si>
-  <si>
-    <t>Build functional interaction with users via Email</t>
-  </si>
-  <si>
-    <t>Trung Hieu Hoang</t>
-  </si>
-  <si>
-    <t>Nhat Huy Huynh Vo</t>
-  </si>
-  <si>
-    <t>Thanh Phong Do + Kien Ba Dau</t>
-  </si>
-  <si>
-    <t>Thanh Lam Do</t>
+    <t>8 day</t>
+  </si>
+  <si>
+    <t>15 day</t>
+  </si>
+  <si>
+    <t>22 day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -233,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -265,24 +211,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -314,7 +247,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -411,6 +367,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -446,6 +419,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -598,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,45 +614,45 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="E1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -670,125 +660,129 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>45</v>
-      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="J3" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="J4" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="J5" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="J6" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="J7" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -796,164 +790,104 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="J8" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>7</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>10</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>11</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" s="11" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:10" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:10" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="1:10" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+    </row>
+    <row r="16" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>